<commit_message>
nptel data analytics (#75)
</commit_message>
<xml_diff>
--- a/ds_ml/ml/1_linear/single_variable/dravid_year_wise_run_1996_to_2011.xlsx
+++ b/ds_ml/ml/1_linear/single_variable/dravid_year_wise_run_1996_to_2011.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -158,10 +158,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -176,6 +176,9 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -184,6 +187,9 @@
       <c r="B2" s="2" t="n">
         <v>436</v>
       </c>
+      <c r="C2" s="2" t="n">
+        <v>436</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -192,6 +198,9 @@
       <c r="B3" s="2" t="n">
         <v>984</v>
       </c>
+      <c r="C3" s="2" t="n">
+        <v>1420</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -200,6 +209,9 @@
       <c r="B4" s="2" t="n">
         <v>413</v>
       </c>
+      <c r="C4" s="2" t="n">
+        <v>1833</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -208,6 +220,9 @@
       <c r="B5" s="2" t="n">
         <v>865</v>
       </c>
+      <c r="C5" s="2" t="n">
+        <v>2698</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -216,6 +231,9 @@
       <c r="B6" s="2" t="n">
         <v>624</v>
       </c>
+      <c r="C6" s="2" t="n">
+        <v>3322</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -224,6 +242,9 @@
       <c r="B7" s="1" t="n">
         <v>935</v>
       </c>
+      <c r="C7" s="2" t="n">
+        <v>4257</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -232,6 +253,9 @@
       <c r="B8" s="2" t="n">
         <v>1375</v>
       </c>
+      <c r="C8" s="2" t="n">
+        <v>5632</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -240,6 +264,9 @@
       <c r="B9" s="2" t="n">
         <v>803</v>
       </c>
+      <c r="C9" s="2" t="n">
+        <v>6435</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -248,6 +275,9 @@
       <c r="B10" s="2" t="n">
         <v>946</v>
       </c>
+      <c r="C10" s="2" t="n">
+        <v>7381</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -256,6 +286,9 @@
       <c r="B11" s="2" t="n">
         <v>640</v>
       </c>
+      <c r="C11" s="2" t="n">
+        <v>8021</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -264,6 +297,9 @@
       <c r="B12" s="2" t="n">
         <v>1095</v>
       </c>
+      <c r="C12" s="2" t="n">
+        <v>9116</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -272,6 +308,9 @@
       <c r="B13" s="2" t="n">
         <v>606</v>
       </c>
+      <c r="C13" s="2" t="n">
+        <v>9722</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -280,6 +319,9 @@
       <c r="B14" s="2" t="n">
         <v>805</v>
       </c>
+      <c r="C14" s="2" t="n">
+        <v>10527</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -288,6 +330,9 @@
       <c r="B15" s="2" t="n">
         <v>747</v>
       </c>
+      <c r="C15" s="2" t="n">
+        <v>11274</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -296,6 +341,9 @@
       <c r="B16" s="2" t="n">
         <v>771</v>
       </c>
+      <c r="C16" s="2" t="n">
+        <v>12045</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -303,6 +351,9 @@
       </c>
       <c r="B17" s="2" t="n">
         <v>1145</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>13190</v>
       </c>
     </row>
   </sheetData>
@@ -324,7 +375,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>